<commit_message>
Updating Trader Quick Risk Workbook
</commit_message>
<xml_diff>
--- a/11 Trader Rules of Thumb/TraderTricks.xlsx
+++ b/11 Trader Rules of Thumb/TraderTricks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\BOOK\.SWAPS_BOOK\11 Trader Pricing Tricks &amp; Rules of Thumb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\BOOK\.SWAPS_BOOK\11 Trader Rules of Thumb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD5A7C1-EF3A-40E1-B04F-85E868C7B750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251E5BB2-798E-4B79-BF74-361F85DE153B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="1380" windowWidth="47160" windowHeight="18600" xr2:uid="{2C45AD73-A93A-4DE3-9C06-A85BD7C29742}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{2C45AD73-A93A-4DE3-9C06-A85BD7C29742}"/>
   </bookViews>
   <sheets>
     <sheet name="Trick 1 - Quick Risk" sheetId="1" r:id="rId1"/>
@@ -651,7 +651,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -711,9 +711,6 @@
     <xf numFmtId="3" fontId="0" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -800,12 +797,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="6" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="6" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="7" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="6" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1321,64 +1312,64 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B2" s="62"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63"/>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63"/>
-      <c r="T2" s="64"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="60"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="61"/>
       <c r="V2" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B3" s="65"/>
-      <c r="C3" s="57" t="s">
+      <c r="B3" s="62"/>
+      <c r="C3" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="57" t="s">
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="58"/>
-      <c r="L3" s="58"/>
-      <c r="M3" s="58"/>
-      <c r="N3" s="58"/>
-      <c r="O3" s="57" t="s">
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="P3" s="58"/>
-      <c r="Q3" s="58"/>
-      <c r="R3" s="57" t="s">
+      <c r="P3" s="55"/>
+      <c r="Q3" s="55"/>
+      <c r="R3" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="S3" s="58"/>
-      <c r="T3" s="66"/>
+      <c r="S3" s="55"/>
+      <c r="T3" s="63"/>
       <c r="V3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B4" s="65"/>
-      <c r="C4" s="59" t="s">
+      <c r="B4" s="62"/>
+      <c r="C4" s="56" t="s">
         <v>20</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -1387,95 +1378,95 @@
       <c r="O4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="P4" s="60"/>
-      <c r="Q4" s="60"/>
+      <c r="P4" s="57"/>
+      <c r="Q4" s="57"/>
       <c r="R4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T4" s="66"/>
-      <c r="V4" s="34"/>
-      <c r="W4" s="34"/>
-      <c r="X4" s="34"/>
-      <c r="Y4" s="34"/>
-      <c r="Z4" s="34"/>
-      <c r="AA4" s="34"/>
+      <c r="T4" s="63"/>
+      <c r="V4" s="33"/>
+      <c r="W4" s="33"/>
+      <c r="X4" s="33"/>
+      <c r="Y4" s="33"/>
+      <c r="Z4" s="33"/>
+      <c r="AA4" s="33"/>
     </row>
     <row r="5" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B5" s="65"/>
-      <c r="D5" s="73" t="s">
+      <c r="B5" s="62"/>
+      <c r="D5" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-      <c r="T5" s="66"/>
-      <c r="V5" s="34"/>
-      <c r="W5" s="34"/>
-      <c r="X5" s="34"/>
-      <c r="Y5" s="34"/>
-      <c r="Z5" s="34"/>
-      <c r="AA5" s="34"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="T5" s="63"/>
+      <c r="V5" s="33"/>
+      <c r="W5" s="33"/>
+      <c r="X5" s="33"/>
+      <c r="Y5" s="33"/>
+      <c r="Z5" s="33"/>
+      <c r="AA5" s="33"/>
     </row>
     <row r="6" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B6" s="65"/>
-      <c r="C6" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="26" t="s">
+      <c r="B6" s="62"/>
+      <c r="C6" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="28" t="s">
+      <c r="H6" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="K6" s="26" t="s">
+      <c r="J6" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="32" t="s">
+      <c r="L6" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="M6" s="33" t="s">
+      <c r="M6" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="N6" s="25"/>
-      <c r="O6" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="P6" s="25" t="s">
+      <c r="N6" s="24"/>
+      <c r="O6" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="P6" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="R6" s="24" t="s">
+      <c r="R6" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="S6" s="25" t="s">
+      <c r="S6" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="T6" s="66"/>
-      <c r="V6" s="34"/>
-      <c r="W6" s="34"/>
-      <c r="X6" s="34"/>
-      <c r="Y6" s="34"/>
-      <c r="Z6" s="34"/>
-      <c r="AA6" s="34"/>
+      <c r="T6" s="63"/>
+      <c r="V6" s="33"/>
+      <c r="W6" s="33"/>
+      <c r="X6" s="33"/>
+      <c r="Y6" s="33"/>
+      <c r="Z6" s="33"/>
+      <c r="AA6" s="33"/>
     </row>
     <row r="7" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B7" s="65"/>
+      <c r="B7" s="62"/>
       <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1506,7 +1497,7 @@
       <c r="M7" s="17">
         <v>0</v>
       </c>
-      <c r="N7" s="25"/>
+      <c r="N7" s="24"/>
       <c r="O7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1520,29 +1511,29 @@
       <c r="S7" s="17">
         <v>0</v>
       </c>
-      <c r="T7" s="66"/>
-      <c r="V7" s="34"/>
-      <c r="W7" s="34"/>
-      <c r="X7" s="34"/>
-      <c r="Y7" s="34"/>
-      <c r="Z7" s="34"/>
-      <c r="AA7" s="34"/>
+      <c r="T7" s="63"/>
+      <c r="V7" s="33"/>
+      <c r="W7" s="33"/>
+      <c r="X7" s="33"/>
+      <c r="Y7" s="33"/>
+      <c r="Z7" s="33"/>
+      <c r="AA7" s="33"/>
     </row>
     <row r="8" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B8" s="65"/>
+      <c r="B8" s="62"/>
       <c r="C8" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="13">
         <v>0</v>
       </c>
-      <c r="E8" s="23">
-        <v>0</v>
-      </c>
-      <c r="F8" s="23">
-        <v>0</v>
-      </c>
-      <c r="G8" s="23">
+      <c r="E8" s="22">
+        <v>0</v>
+      </c>
+      <c r="F8" s="22">
+        <v>0</v>
+      </c>
+      <c r="G8" s="22">
         <v>0</v>
       </c>
       <c r="H8" s="14">
@@ -1554,13 +1545,13 @@
       <c r="K8" s="13">
         <v>0</v>
       </c>
-      <c r="L8" s="23">
+      <c r="L8" s="22">
         <v>0</v>
       </c>
       <c r="M8" s="14">
         <v>0</v>
       </c>
-      <c r="N8" s="25"/>
+      <c r="N8" s="24"/>
       <c r="O8" s="6" t="s">
         <v>7</v>
       </c>
@@ -1574,16 +1565,16 @@
       <c r="S8" s="14">
         <v>0</v>
       </c>
-      <c r="T8" s="66"/>
-      <c r="V8" s="34"/>
-      <c r="W8" s="34"/>
-      <c r="X8" s="34"/>
-      <c r="Y8" s="34"/>
-      <c r="Z8" s="34"/>
-      <c r="AA8" s="34"/>
+      <c r="T8" s="63"/>
+      <c r="V8" s="33"/>
+      <c r="W8" s="33"/>
+      <c r="X8" s="33"/>
+      <c r="Y8" s="33"/>
+      <c r="Z8" s="33"/>
+      <c r="AA8" s="33"/>
     </row>
     <row r="9" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B9" s="65"/>
+      <c r="B9" s="62"/>
       <c r="C9" s="5" t="s">
         <v>8</v>
       </c>
@@ -1614,7 +1605,7 @@
       <c r="M9" s="17">
         <v>0</v>
       </c>
-      <c r="N9" s="25"/>
+      <c r="N9" s="24"/>
       <c r="O9" s="6" t="s">
         <v>8</v>
       </c>
@@ -1628,29 +1619,29 @@
       <c r="S9" s="17">
         <v>0</v>
       </c>
-      <c r="T9" s="66"/>
-      <c r="V9" s="34"/>
-      <c r="W9" s="34"/>
-      <c r="X9" s="34"/>
-      <c r="Y9" s="34"/>
-      <c r="Z9" s="34"/>
-      <c r="AA9" s="34"/>
+      <c r="T9" s="63"/>
+      <c r="V9" s="33"/>
+      <c r="W9" s="33"/>
+      <c r="X9" s="33"/>
+      <c r="Y9" s="33"/>
+      <c r="Z9" s="33"/>
+      <c r="AA9" s="33"/>
     </row>
     <row r="10" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B10" s="65"/>
+      <c r="B10" s="62"/>
       <c r="C10" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="13">
         <v>0</v>
       </c>
-      <c r="E10" s="23">
-        <v>0</v>
-      </c>
-      <c r="F10" s="23">
-        <v>0</v>
-      </c>
-      <c r="G10" s="23">
+      <c r="E10" s="22">
+        <v>0</v>
+      </c>
+      <c r="F10" s="22">
+        <v>0</v>
+      </c>
+      <c r="G10" s="22">
         <v>0</v>
       </c>
       <c r="H10" s="14">
@@ -1662,13 +1653,13 @@
       <c r="K10" s="13">
         <v>0</v>
       </c>
-      <c r="L10" s="23">
+      <c r="L10" s="22">
         <v>0</v>
       </c>
       <c r="M10" s="14">
         <v>0</v>
       </c>
-      <c r="N10" s="25"/>
+      <c r="N10" s="24"/>
       <c r="O10" s="6" t="s">
         <v>9</v>
       </c>
@@ -1682,16 +1673,16 @@
       <c r="S10" s="14">
         <v>0</v>
       </c>
-      <c r="T10" s="66"/>
-      <c r="V10" s="34"/>
-      <c r="W10" s="34"/>
-      <c r="X10" s="34"/>
-      <c r="Y10" s="34"/>
-      <c r="Z10" s="34"/>
-      <c r="AA10" s="34"/>
+      <c r="T10" s="63"/>
+      <c r="V10" s="33"/>
+      <c r="W10" s="33"/>
+      <c r="X10" s="33"/>
+      <c r="Y10" s="33"/>
+      <c r="Z10" s="33"/>
+      <c r="AA10" s="33"/>
     </row>
     <row r="11" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B11" s="65"/>
+      <c r="B11" s="62"/>
       <c r="C11" s="5" t="s">
         <v>10</v>
       </c>
@@ -1722,7 +1713,7 @@
       <c r="M11" s="17">
         <v>0</v>
       </c>
-      <c r="N11" s="25"/>
+      <c r="N11" s="24"/>
       <c r="O11" s="6" t="s">
         <v>10</v>
       </c>
@@ -1736,29 +1727,29 @@
       <c r="S11" s="17">
         <v>0</v>
       </c>
-      <c r="T11" s="66"/>
-      <c r="V11" s="34"/>
-      <c r="W11" s="34"/>
-      <c r="X11" s="34"/>
-      <c r="Y11" s="34"/>
-      <c r="Z11" s="34"/>
-      <c r="AA11" s="34"/>
+      <c r="T11" s="63"/>
+      <c r="V11" s="33"/>
+      <c r="W11" s="33"/>
+      <c r="X11" s="33"/>
+      <c r="Y11" s="33"/>
+      <c r="Z11" s="33"/>
+      <c r="AA11" s="33"/>
     </row>
     <row r="12" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B12" s="65"/>
+      <c r="B12" s="62"/>
       <c r="C12" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="13">
         <v>98.228077410510949</v>
       </c>
-      <c r="E12" s="23">
-        <v>0</v>
-      </c>
-      <c r="F12" s="23">
+      <c r="E12" s="22">
+        <v>0</v>
+      </c>
+      <c r="F12" s="22">
         <v>1.6151139266262924E-14</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="22">
         <v>2.1400131077185563E-14</v>
       </c>
       <c r="H12" s="14">
@@ -1770,13 +1761,13 @@
       <c r="K12" s="13">
         <v>98.228077410510949</v>
       </c>
-      <c r="L12" s="23">
+      <c r="L12" s="22">
         <v>-2.1400131077185566E-14</v>
       </c>
       <c r="M12" s="14">
         <v>1.070006553859278E-14</v>
       </c>
-      <c r="N12" s="25"/>
+      <c r="N12" s="24"/>
       <c r="O12" s="6" t="s">
         <v>11</v>
       </c>
@@ -1787,20 +1778,20 @@
       <c r="R12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="S12" s="22">
+      <c r="S12" s="14">
         <f>-P12/$D$20</f>
         <v>-0.99999999999999989</v>
       </c>
-      <c r="T12" s="66"/>
-      <c r="V12" s="34"/>
-      <c r="W12" s="34"/>
-      <c r="X12" s="34"/>
-      <c r="Y12" s="34"/>
-      <c r="Z12" s="34"/>
-      <c r="AA12" s="34"/>
+      <c r="T12" s="63"/>
+      <c r="V12" s="33"/>
+      <c r="W12" s="33"/>
+      <c r="X12" s="33"/>
+      <c r="Y12" s="33"/>
+      <c r="Z12" s="33"/>
+      <c r="AA12" s="33"/>
     </row>
     <row r="13" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B13" s="65"/>
+      <c r="B13" s="62"/>
       <c r="C13" s="5" t="s">
         <v>12</v>
       </c>
@@ -1831,7 +1822,7 @@
       <c r="M13" s="17">
         <v>-1.4395052561247795E-13</v>
       </c>
-      <c r="N13" s="25"/>
+      <c r="N13" s="24"/>
       <c r="O13" s="6" t="s">
         <v>12</v>
       </c>
@@ -1846,29 +1837,29 @@
         <f>-P13/$E$20</f>
         <v>4.6515163384814275E-16</v>
       </c>
-      <c r="T13" s="66"/>
-      <c r="V13" s="34"/>
-      <c r="W13" s="34"/>
-      <c r="X13" s="34"/>
-      <c r="Y13" s="34"/>
-      <c r="Z13" s="34"/>
-      <c r="AA13" s="34"/>
+      <c r="T13" s="63"/>
+      <c r="V13" s="33"/>
+      <c r="W13" s="33"/>
+      <c r="X13" s="33"/>
+      <c r="Y13" s="33"/>
+      <c r="Z13" s="33"/>
+      <c r="AA13" s="33"/>
     </row>
     <row r="14" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B14" s="65"/>
+      <c r="B14" s="62"/>
       <c r="C14" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="13">
         <v>0</v>
       </c>
-      <c r="E14" s="23">
-        <v>0</v>
-      </c>
-      <c r="F14" s="23">
+      <c r="E14" s="22">
+        <v>0</v>
+      </c>
+      <c r="F14" s="22">
         <v>290.95305912460276</v>
       </c>
-      <c r="G14" s="23">
+      <c r="G14" s="22">
         <v>5.6843418860808015E-14</v>
       </c>
       <c r="H14" s="14">
@@ -1880,13 +1871,13 @@
       <c r="K14" s="13">
         <v>0</v>
       </c>
-      <c r="L14" s="23">
+      <c r="L14" s="22">
         <v>-5.3159461939892194E-14</v>
       </c>
       <c r="M14" s="14">
         <v>3.0263687890861921E-14</v>
       </c>
-      <c r="N14" s="25"/>
+      <c r="N14" s="24"/>
       <c r="O14" s="6" t="s">
         <v>13</v>
       </c>
@@ -1901,16 +1892,16 @@
         <f>-P14/$F$20</f>
         <v>7.8692329676537289E-17</v>
       </c>
-      <c r="T14" s="66"/>
-      <c r="V14" s="34"/>
-      <c r="W14" s="34"/>
-      <c r="X14" s="34"/>
-      <c r="Y14" s="34"/>
-      <c r="Z14" s="34"/>
-      <c r="AA14" s="34"/>
+      <c r="T14" s="63"/>
+      <c r="V14" s="33"/>
+      <c r="W14" s="33"/>
+      <c r="X14" s="33"/>
+      <c r="Y14" s="33"/>
+      <c r="Z14" s="33"/>
+      <c r="AA14" s="33"/>
     </row>
     <row r="15" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B15" s="65"/>
+      <c r="B15" s="62"/>
       <c r="C15" s="5" t="s">
         <v>14</v>
       </c>
@@ -1941,7 +1932,7 @@
       <c r="M15" s="17">
         <v>192.75524468978531</v>
       </c>
-      <c r="N15" s="25"/>
+      <c r="N15" s="24"/>
       <c r="O15" s="6" t="s">
         <v>14</v>
       </c>
@@ -1952,51 +1943,51 @@
       <c r="R15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="S15" s="21">
-        <f>-G15/$G$20</f>
-        <v>-1.0000000000000002</v>
-      </c>
-      <c r="T15" s="66"/>
-      <c r="V15" s="34"/>
-      <c r="W15" s="34"/>
-      <c r="X15" s="34"/>
-      <c r="Y15" s="34"/>
-      <c r="Z15" s="34"/>
-      <c r="AA15" s="34"/>
+      <c r="S15" s="17">
+        <f>-P15/$G$20</f>
+        <v>0.50000000000000011</v>
+      </c>
+      <c r="T15" s="63"/>
+      <c r="V15" s="33"/>
+      <c r="W15" s="33"/>
+      <c r="X15" s="33"/>
+      <c r="Y15" s="33"/>
+      <c r="Z15" s="33"/>
+      <c r="AA15" s="33"/>
     </row>
     <row r="16" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B16" s="65"/>
+      <c r="B16" s="62"/>
       <c r="C16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="29">
-        <v>0</v>
-      </c>
-      <c r="E16" s="30">
-        <v>0</v>
-      </c>
-      <c r="F16" s="30">
-        <v>0</v>
-      </c>
-      <c r="G16" s="30">
-        <v>0</v>
-      </c>
-      <c r="H16" s="31">
+      <c r="D16" s="28">
+        <v>0</v>
+      </c>
+      <c r="E16" s="29">
+        <v>0</v>
+      </c>
+      <c r="F16" s="29">
+        <v>0</v>
+      </c>
+      <c r="G16" s="29">
+        <v>0</v>
+      </c>
+      <c r="H16" s="30">
         <v>478.8178659674291</v>
       </c>
       <c r="J16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="K16" s="29">
-        <v>0</v>
-      </c>
-      <c r="L16" s="30">
+      <c r="K16" s="28">
+        <v>0</v>
+      </c>
+      <c r="L16" s="29">
         <v>478.8178659674291</v>
       </c>
-      <c r="M16" s="31">
+      <c r="M16" s="30">
         <v>239.40893298371455</v>
       </c>
-      <c r="N16" s="25"/>
+      <c r="N16" s="24"/>
       <c r="O16" s="9" t="s">
         <v>15</v>
       </c>
@@ -2007,22 +1998,22 @@
       <c r="R16" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="S16" s="22">
+      <c r="S16" s="21">
         <f>-P16/$H$20</f>
         <v>-1.5000000000000004</v>
       </c>
-      <c r="T16" s="66"/>
+      <c r="T16" s="63"/>
     </row>
     <row r="17" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B17" s="65"/>
-      <c r="N17" s="25"/>
-      <c r="T17" s="66"/>
+      <c r="B17" s="62"/>
+      <c r="N17" s="24"/>
+      <c r="T17" s="63"/>
       <c r="V17" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B18" s="65"/>
+      <c r="B18" s="62"/>
       <c r="D18" s="1" t="s">
         <v>16</v>
       </c>
@@ -2030,32 +2021,32 @@
         <v>16</v>
       </c>
       <c r="L18" s="1"/>
-      <c r="N18" s="25"/>
-      <c r="T18" s="66"/>
-      <c r="V18" s="34"/>
-      <c r="W18" s="34"/>
-      <c r="X18" s="34"/>
-      <c r="Y18" s="34"/>
-      <c r="Z18" s="34"/>
+      <c r="N18" s="24"/>
+      <c r="T18" s="63"/>
+      <c r="V18" s="33"/>
+      <c r="W18" s="33"/>
+      <c r="X18" s="33"/>
+      <c r="Y18" s="33"/>
+      <c r="Z18" s="33"/>
     </row>
     <row r="19" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B19" s="65"/>
-      <c r="D19" s="26" t="s">
+      <c r="B19" s="62"/>
+      <c r="D19" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="27" t="s">
+      <c r="E19" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="27" t="s">
+      <c r="F19" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="27" t="s">
+      <c r="G19" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="28" t="s">
+      <c r="H19" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="K19" s="26" t="s">
+      <c r="K19" s="25" t="s">
         <v>11</v>
       </c>
       <c r="L19" s="11" t="s">
@@ -2064,20 +2055,20 @@
       <c r="M19" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="N19" s="25"/>
-      <c r="O19" s="25"/>
-      <c r="P19" s="61" t="s">
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="T19" s="66"/>
-      <c r="V19" s="34"/>
-      <c r="W19" s="34"/>
-      <c r="X19" s="34"/>
-      <c r="Y19" s="34"/>
-      <c r="Z19" s="34"/>
+      <c r="T19" s="63"/>
+      <c r="V19" s="33"/>
+      <c r="W19" s="33"/>
+      <c r="X19" s="33"/>
+      <c r="Y19" s="33"/>
+      <c r="Z19" s="33"/>
     </row>
     <row r="20" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B20" s="65"/>
+      <c r="B20" s="62"/>
       <c r="D20" s="18">
         <f t="shared" ref="D20:M20" si="1">SUM(D7:D16)</f>
         <v>98.228077410510949</v>
@@ -2110,107 +2101,107 @@
         <f t="shared" si="1"/>
         <v>432.16417767349975</v>
       </c>
-      <c r="N20" s="25"/>
+      <c r="N20" s="24"/>
       <c r="P20" s="20">
         <f>SUM(P7:P16)</f>
         <v>623.69963167186916</v>
       </c>
-      <c r="T20" s="66"/>
-      <c r="V20" s="34"/>
-      <c r="W20" s="34"/>
-      <c r="X20" s="34"/>
-      <c r="Y20" s="34"/>
-      <c r="Z20" s="34"/>
+      <c r="T20" s="63"/>
+      <c r="V20" s="33"/>
+      <c r="W20" s="33"/>
+      <c r="X20" s="33"/>
+      <c r="Y20" s="33"/>
+      <c r="Z20" s="33"/>
     </row>
     <row r="21" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B21" s="65"/>
-      <c r="T21" s="66"/>
+      <c r="B21" s="62"/>
+      <c r="T21" s="63"/>
     </row>
     <row r="22" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B22" s="67"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="68"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="68"/>
-      <c r="H22" s="68"/>
-      <c r="I22" s="68"/>
-      <c r="J22" s="68"/>
-      <c r="K22" s="68"/>
-      <c r="L22" s="68"/>
-      <c r="M22" s="68"/>
-      <c r="N22" s="69"/>
-      <c r="O22" s="68"/>
-      <c r="P22" s="68"/>
-      <c r="Q22" s="68"/>
-      <c r="R22" s="68"/>
-      <c r="S22" s="68"/>
-      <c r="T22" s="70"/>
+      <c r="B22" s="64"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="65"/>
+      <c r="H22" s="65"/>
+      <c r="I22" s="65"/>
+      <c r="J22" s="65"/>
+      <c r="K22" s="65"/>
+      <c r="L22" s="65"/>
+      <c r="M22" s="65"/>
+      <c r="N22" s="66"/>
+      <c r="O22" s="65"/>
+      <c r="P22" s="65"/>
+      <c r="Q22" s="65"/>
+      <c r="R22" s="65"/>
+      <c r="S22" s="65"/>
+      <c r="T22" s="67"/>
       <c r="V22" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="23" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B23" s="62"/>
-      <c r="C23" s="63"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="63"/>
-      <c r="F23" s="63"/>
-      <c r="G23" s="63"/>
-      <c r="H23" s="63"/>
-      <c r="I23" s="63"/>
-      <c r="J23" s="63"/>
-      <c r="K23" s="63"/>
-      <c r="L23" s="63"/>
-      <c r="M23" s="63"/>
-      <c r="N23" s="63"/>
-      <c r="O23" s="63"/>
-      <c r="P23" s="63"/>
-      <c r="Q23" s="63"/>
-      <c r="R23" s="63"/>
-      <c r="S23" s="63"/>
-      <c r="T23" s="64"/>
-      <c r="V23" s="34"/>
-      <c r="W23" s="34"/>
-      <c r="X23" s="34"/>
-      <c r="Y23" s="34"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="60"/>
+      <c r="I23" s="60"/>
+      <c r="J23" s="60"/>
+      <c r="K23" s="60"/>
+      <c r="L23" s="60"/>
+      <c r="M23" s="60"/>
+      <c r="N23" s="60"/>
+      <c r="O23" s="60"/>
+      <c r="P23" s="60"/>
+      <c r="Q23" s="60"/>
+      <c r="R23" s="60"/>
+      <c r="S23" s="60"/>
+      <c r="T23" s="61"/>
+      <c r="V23" s="33"/>
+      <c r="W23" s="33"/>
+      <c r="X23" s="33"/>
+      <c r="Y23" s="33"/>
     </row>
     <row r="24" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B24" s="65"/>
-      <c r="C24" s="71" t="s">
+      <c r="B24" s="62"/>
+      <c r="C24" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="72"/>
-      <c r="E24" s="72"/>
-      <c r="F24" s="72"/>
-      <c r="G24" s="72"/>
-      <c r="H24" s="72"/>
-      <c r="I24" s="72"/>
-      <c r="J24" s="71" t="s">
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="69"/>
+      <c r="H24" s="69"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="K24" s="72"/>
-      <c r="L24" s="72"/>
-      <c r="M24" s="72"/>
-      <c r="N24" s="72"/>
-      <c r="O24" s="71" t="s">
+      <c r="K24" s="69"/>
+      <c r="L24" s="69"/>
+      <c r="M24" s="69"/>
+      <c r="N24" s="69"/>
+      <c r="O24" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="P24" s="72"/>
-      <c r="Q24" s="72"/>
-      <c r="R24" s="71" t="s">
+      <c r="P24" s="69"/>
+      <c r="Q24" s="69"/>
+      <c r="R24" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="S24" s="72"/>
-      <c r="T24" s="66"/>
-      <c r="V24" s="34"/>
-      <c r="W24" s="34"/>
-      <c r="X24" s="34"/>
-      <c r="Y24" s="34"/>
+      <c r="S24" s="69"/>
+      <c r="T24" s="63"/>
+      <c r="V24" s="33"/>
+      <c r="W24" s="33"/>
+      <c r="X24" s="33"/>
+      <c r="Y24" s="33"/>
     </row>
     <row r="25" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B25" s="65"/>
-      <c r="C25" s="59" t="s">
+      <c r="B25" s="62"/>
+      <c r="C25" s="56" t="s">
         <v>20</v>
       </c>
       <c r="J25" s="1" t="s">
@@ -2219,581 +2210,581 @@
       <c r="O25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="P25" s="60"/>
-      <c r="Q25" s="60"/>
+      <c r="P25" s="57"/>
+      <c r="Q25" s="57"/>
       <c r="R25" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T25" s="66"/>
-      <c r="V25" s="34"/>
-      <c r="W25" s="34"/>
-      <c r="X25" s="34"/>
-      <c r="Y25" s="34"/>
+      <c r="T25" s="63"/>
+      <c r="V25" s="33"/>
+      <c r="W25" s="33"/>
+      <c r="X25" s="33"/>
+      <c r="Y25" s="33"/>
     </row>
     <row r="26" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B26" s="65"/>
-      <c r="D26" s="24" t="s">
+      <c r="B26" s="62"/>
+      <c r="D26" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="T26" s="66"/>
-      <c r="V26" s="34"/>
-      <c r="W26" s="34"/>
-      <c r="X26" s="34"/>
-      <c r="Y26" s="34"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="T26" s="63"/>
+      <c r="V26" s="33"/>
+      <c r="W26" s="33"/>
+      <c r="X26" s="33"/>
+      <c r="Y26" s="33"/>
     </row>
     <row r="27" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B27" s="65"/>
-      <c r="C27" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="D27" s="26" t="s">
+      <c r="B27" s="62"/>
+      <c r="C27" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="F27" s="27" t="s">
+      <c r="F27" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="27" t="s">
+      <c r="G27" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="H27" s="28" t="s">
+      <c r="H27" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="J27" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="K27" s="26" t="s">
+      <c r="J27" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="K27" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="L27" s="32" t="s">
+      <c r="L27" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="M27" s="33" t="s">
+      <c r="M27" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="N27" s="25"/>
-      <c r="O27" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="P27" s="25" t="s">
+      <c r="N27" s="24"/>
+      <c r="O27" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="P27" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="R27" s="24" t="s">
+      <c r="R27" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="S27" s="25" t="s">
+      <c r="S27" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="T27" s="66"/>
-      <c r="V27" s="34"/>
-      <c r="W27" s="34"/>
-      <c r="X27" s="34"/>
-      <c r="Y27" s="34"/>
+      <c r="T27" s="63"/>
+      <c r="V27" s="33"/>
+      <c r="W27" s="33"/>
+      <c r="X27" s="33"/>
+      <c r="Y27" s="33"/>
     </row>
     <row r="28" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B28" s="65"/>
+      <c r="B28" s="62"/>
       <c r="C28" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="38">
-        <v>0</v>
-      </c>
-      <c r="E28" s="39">
-        <v>0</v>
-      </c>
-      <c r="F28" s="39">
-        <v>0</v>
-      </c>
-      <c r="G28" s="39">
-        <v>0</v>
-      </c>
-      <c r="H28" s="40">
+      <c r="D28" s="37">
+        <v>0</v>
+      </c>
+      <c r="E28" s="38">
+        <v>0</v>
+      </c>
+      <c r="F28" s="38">
+        <v>0</v>
+      </c>
+      <c r="G28" s="38">
+        <v>0</v>
+      </c>
+      <c r="H28" s="39">
         <v>0</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K28" s="41">
-        <v>0</v>
-      </c>
-      <c r="L28" s="42">
-        <v>0</v>
-      </c>
-      <c r="M28" s="43">
-        <v>0</v>
-      </c>
-      <c r="N28" s="25"/>
+      <c r="K28" s="40">
+        <v>0</v>
+      </c>
+      <c r="L28" s="41">
+        <v>0</v>
+      </c>
+      <c r="M28" s="42">
+        <v>0</v>
+      </c>
+      <c r="N28" s="24"/>
       <c r="O28" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="P28" s="43">
+      <c r="P28" s="42">
         <f t="shared" ref="P28:P37" si="3">SUM(K28:M28)</f>
         <v>0</v>
       </c>
       <c r="R28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="S28" s="43">
-        <v>0</v>
-      </c>
-      <c r="T28" s="66"/>
-      <c r="V28" s="34"/>
-      <c r="W28" s="34"/>
-      <c r="X28" s="34"/>
-      <c r="Y28" s="34"/>
+      <c r="S28" s="42">
+        <v>0</v>
+      </c>
+      <c r="T28" s="63"/>
+      <c r="V28" s="33"/>
+      <c r="W28" s="33"/>
+      <c r="X28" s="33"/>
+      <c r="Y28" s="33"/>
     </row>
     <row r="29" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B29" s="65"/>
+      <c r="B29" s="62"/>
       <c r="C29" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="35">
-        <v>0</v>
-      </c>
-      <c r="E29" s="36">
-        <v>0</v>
-      </c>
-      <c r="F29" s="36">
-        <v>0</v>
-      </c>
-      <c r="G29" s="36">
-        <v>0</v>
-      </c>
-      <c r="H29" s="37">
+      <c r="D29" s="34">
+        <v>0</v>
+      </c>
+      <c r="E29" s="35">
+        <v>0</v>
+      </c>
+      <c r="F29" s="35">
+        <v>0</v>
+      </c>
+      <c r="G29" s="35">
+        <v>0</v>
+      </c>
+      <c r="H29" s="36">
         <v>0</v>
       </c>
       <c r="J29" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="K29" s="44">
-        <v>0</v>
-      </c>
-      <c r="L29" s="36">
-        <v>0</v>
-      </c>
-      <c r="M29" s="45">
-        <v>0</v>
-      </c>
-      <c r="N29" s="25"/>
+      <c r="K29" s="43">
+        <v>0</v>
+      </c>
+      <c r="L29" s="35">
+        <v>0</v>
+      </c>
+      <c r="M29" s="44">
+        <v>0</v>
+      </c>
+      <c r="N29" s="24"/>
       <c r="O29" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="P29" s="45">
+      <c r="P29" s="44">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R29" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="S29" s="45">
-        <v>0</v>
-      </c>
-      <c r="T29" s="66"/>
+      <c r="S29" s="44">
+        <v>0</v>
+      </c>
+      <c r="T29" s="63"/>
     </row>
     <row r="30" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B30" s="65"/>
+      <c r="B30" s="62"/>
       <c r="C30" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="38">
-        <v>0</v>
-      </c>
-      <c r="E30" s="39">
-        <v>0</v>
-      </c>
-      <c r="F30" s="39">
-        <v>0</v>
-      </c>
-      <c r="G30" s="39">
-        <v>0</v>
-      </c>
-      <c r="H30" s="40">
+      <c r="D30" s="37">
+        <v>0</v>
+      </c>
+      <c r="E30" s="38">
+        <v>0</v>
+      </c>
+      <c r="F30" s="38">
+        <v>0</v>
+      </c>
+      <c r="G30" s="38">
+        <v>0</v>
+      </c>
+      <c r="H30" s="39">
         <v>0</v>
       </c>
       <c r="J30" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K30" s="46">
-        <v>0</v>
-      </c>
-      <c r="L30" s="47">
-        <v>0</v>
-      </c>
-      <c r="M30" s="48">
-        <v>0</v>
-      </c>
-      <c r="N30" s="25"/>
+      <c r="K30" s="45">
+        <v>0</v>
+      </c>
+      <c r="L30" s="46">
+        <v>0</v>
+      </c>
+      <c r="M30" s="47">
+        <v>0</v>
+      </c>
+      <c r="N30" s="24"/>
       <c r="O30" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="P30" s="48">
+      <c r="P30" s="47">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R30" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="S30" s="48">
-        <v>0</v>
-      </c>
-      <c r="T30" s="66"/>
+      <c r="S30" s="47">
+        <v>0</v>
+      </c>
+      <c r="T30" s="63"/>
     </row>
     <row r="31" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B31" s="65"/>
+      <c r="B31" s="62"/>
       <c r="C31" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D31" s="35">
-        <v>0</v>
-      </c>
-      <c r="E31" s="36">
-        <v>0</v>
-      </c>
-      <c r="F31" s="36">
-        <v>0</v>
-      </c>
-      <c r="G31" s="36">
-        <v>0</v>
-      </c>
-      <c r="H31" s="37">
+      <c r="D31" s="34">
+        <v>0</v>
+      </c>
+      <c r="E31" s="35">
+        <v>0</v>
+      </c>
+      <c r="F31" s="35">
+        <v>0</v>
+      </c>
+      <c r="G31" s="35">
+        <v>0</v>
+      </c>
+      <c r="H31" s="36">
         <v>0</v>
       </c>
       <c r="J31" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K31" s="44">
-        <v>0</v>
-      </c>
-      <c r="L31" s="36">
-        <v>0</v>
-      </c>
-      <c r="M31" s="45">
-        <v>0</v>
-      </c>
-      <c r="N31" s="25"/>
+      <c r="K31" s="43">
+        <v>0</v>
+      </c>
+      <c r="L31" s="35">
+        <v>0</v>
+      </c>
+      <c r="M31" s="44">
+        <v>0</v>
+      </c>
+      <c r="N31" s="24"/>
       <c r="O31" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="P31" s="45">
+      <c r="P31" s="44">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R31" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="S31" s="45">
-        <v>0</v>
-      </c>
-      <c r="T31" s="66"/>
+      <c r="S31" s="44">
+        <v>0</v>
+      </c>
+      <c r="T31" s="63"/>
     </row>
     <row r="32" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B32" s="65"/>
+      <c r="B32" s="62"/>
       <c r="C32" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D32" s="38">
-        <v>0</v>
-      </c>
-      <c r="E32" s="39">
-        <v>0</v>
-      </c>
-      <c r="F32" s="39">
-        <v>0</v>
-      </c>
-      <c r="G32" s="39">
-        <v>0</v>
-      </c>
-      <c r="H32" s="40">
+      <c r="D32" s="37">
+        <v>0</v>
+      </c>
+      <c r="E32" s="38">
+        <v>0</v>
+      </c>
+      <c r="F32" s="38">
+        <v>0</v>
+      </c>
+      <c r="G32" s="38">
+        <v>0</v>
+      </c>
+      <c r="H32" s="39">
         <v>0</v>
       </c>
       <c r="J32" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K32" s="46">
-        <v>0</v>
-      </c>
-      <c r="L32" s="47">
-        <v>0</v>
-      </c>
-      <c r="M32" s="48">
-        <v>0</v>
-      </c>
-      <c r="N32" s="25"/>
+      <c r="K32" s="45">
+        <v>0</v>
+      </c>
+      <c r="L32" s="46">
+        <v>0</v>
+      </c>
+      <c r="M32" s="47">
+        <v>0</v>
+      </c>
+      <c r="N32" s="24"/>
       <c r="O32" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="P32" s="48">
+      <c r="P32" s="47">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R32" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="S32" s="48">
-        <v>0</v>
-      </c>
-      <c r="T32" s="66"/>
+      <c r="S32" s="47">
+        <v>0</v>
+      </c>
+      <c r="T32" s="63"/>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B33" s="65"/>
+      <c r="B33" s="62"/>
       <c r="C33" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D33" s="35">
+      <c r="D33" s="34">
         <v>100</v>
       </c>
-      <c r="E33" s="36">
-        <v>0</v>
-      </c>
-      <c r="F33" s="36">
+      <c r="E33" s="35">
+        <v>0</v>
+      </c>
+      <c r="F33" s="35">
         <v>1.6151139266262924E-14</v>
       </c>
-      <c r="G33" s="36">
+      <c r="G33" s="35">
         <v>2.1400131077185563E-14</v>
       </c>
-      <c r="H33" s="37">
+      <c r="H33" s="36">
         <v>-3.1554436208840472E-30</v>
       </c>
       <c r="J33" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K33" s="44">
+      <c r="K33" s="43">
         <v>100</v>
       </c>
-      <c r="L33" s="36">
+      <c r="L33" s="35">
         <v>-2.1400131077185566E-14</v>
       </c>
-      <c r="M33" s="45">
+      <c r="M33" s="44">
         <v>1.070006553859278E-14</v>
       </c>
-      <c r="N33" s="25"/>
+      <c r="N33" s="24"/>
       <c r="O33" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="P33" s="45">
+      <c r="P33" s="44">
         <f t="shared" si="3"/>
         <v>99.999999999999986</v>
       </c>
       <c r="R33" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="S33" s="52">
+      <c r="S33" s="44">
         <f>-P33/$D$41</f>
         <v>-0.99999999999999989</v>
       </c>
-      <c r="T33" s="66"/>
+      <c r="T33" s="63"/>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B34" s="65"/>
+      <c r="B34" s="62"/>
       <c r="C34" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D34" s="38">
-        <v>0</v>
-      </c>
-      <c r="E34" s="39">
+      <c r="D34" s="37">
+        <v>0</v>
+      </c>
+      <c r="E34" s="38">
         <v>200</v>
       </c>
-      <c r="F34" s="39">
+      <c r="F34" s="38">
         <v>-1.7053025658242404E-13</v>
       </c>
-      <c r="G34" s="39">
+      <c r="G34" s="38">
         <v>-1.7053025658242404E-13</v>
       </c>
-      <c r="H34" s="40">
+      <c r="H34" s="39">
         <v>-1.1737079464253186E-13</v>
       </c>
       <c r="J34" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K34" s="46">
-        <v>0</v>
-      </c>
-      <c r="L34" s="47">
+      <c r="K34" s="45">
+        <v>0</v>
+      </c>
+      <c r="L34" s="46">
         <v>5.3159461939892194E-14</v>
       </c>
-      <c r="M34" s="48">
+      <c r="M34" s="47">
         <v>-1.4395052561247795E-13</v>
       </c>
-      <c r="N34" s="25"/>
+      <c r="N34" s="24"/>
       <c r="O34" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="P34" s="48">
+      <c r="P34" s="47">
         <f t="shared" si="3"/>
         <v>-9.0791063672585763E-14</v>
       </c>
       <c r="R34" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="S34" s="48">
+      <c r="S34" s="47">
         <f>-P34/$E$41</f>
         <v>4.5395531836292877E-16</v>
       </c>
-      <c r="T34" s="66"/>
+      <c r="T34" s="63"/>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B35" s="65"/>
+      <c r="B35" s="62"/>
       <c r="C35" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="35">
-        <v>0</v>
-      </c>
-      <c r="E35" s="36">
-        <v>0</v>
-      </c>
-      <c r="F35" s="36">
+      <c r="D35" s="34">
+        <v>0</v>
+      </c>
+      <c r="E35" s="35">
+        <v>0</v>
+      </c>
+      <c r="F35" s="35">
         <v>300</v>
       </c>
-      <c r="G35" s="36">
+      <c r="G35" s="35">
         <v>5.6843418860808015E-14</v>
       </c>
-      <c r="H35" s="37">
+      <c r="H35" s="36">
         <v>3.6839569209158207E-15</v>
       </c>
       <c r="J35" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K35" s="44">
-        <v>0</v>
-      </c>
-      <c r="L35" s="36">
+      <c r="K35" s="43">
+        <v>0</v>
+      </c>
+      <c r="L35" s="35">
         <v>-5.3159461939892194E-14</v>
       </c>
-      <c r="M35" s="45">
+      <c r="M35" s="44">
         <v>3.0263687890861921E-14</v>
       </c>
-      <c r="N35" s="25"/>
+      <c r="N35" s="24"/>
       <c r="O35" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="P35" s="45">
+      <c r="P35" s="44">
         <f t="shared" si="3"/>
         <v>-2.2895774049030273E-14</v>
       </c>
       <c r="R35" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="S35" s="45">
+      <c r="S35" s="44">
         <f>-P35/$F$41</f>
         <v>7.6319246830100959E-17</v>
       </c>
-      <c r="T35" s="66"/>
+      <c r="T35" s="63"/>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B36" s="65"/>
+      <c r="B36" s="62"/>
       <c r="C36" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="38">
-        <v>0</v>
-      </c>
-      <c r="E36" s="39">
-        <v>0</v>
-      </c>
-      <c r="F36" s="39">
-        <v>0</v>
-      </c>
-      <c r="G36" s="39">
+      <c r="D36" s="37">
+        <v>0</v>
+      </c>
+      <c r="E36" s="38">
+        <v>0</v>
+      </c>
+      <c r="F36" s="38">
+        <v>0</v>
+      </c>
+      <c r="G36" s="38">
         <v>400</v>
       </c>
-      <c r="H36" s="40">
+      <c r="H36" s="39">
         <v>0</v>
       </c>
       <c r="J36" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K36" s="46">
-        <v>0</v>
-      </c>
-      <c r="L36" s="47">
+      <c r="K36" s="45">
+        <v>0</v>
+      </c>
+      <c r="L36" s="46">
         <v>-400</v>
       </c>
-      <c r="M36" s="48">
+      <c r="M36" s="47">
         <f>50%*400</f>
         <v>200</v>
       </c>
-      <c r="N36" s="25"/>
+      <c r="N36" s="24"/>
       <c r="O36" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P36" s="48">
+      <c r="P36" s="47">
         <f t="shared" si="3"/>
         <v>-200</v>
       </c>
       <c r="R36" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="S36" s="53">
-        <f>-G36/$G$41</f>
-        <v>-1.0000000000000002</v>
-      </c>
-      <c r="T36" s="66"/>
+      <c r="S36" s="47">
+        <f>-P36/$G$41</f>
+        <v>0.50000000000000011</v>
+      </c>
+      <c r="T36" s="63"/>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B37" s="65"/>
+      <c r="B37" s="62"/>
       <c r="C37" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D37" s="35">
-        <v>0</v>
-      </c>
-      <c r="E37" s="36">
-        <v>0</v>
-      </c>
-      <c r="F37" s="36">
-        <v>0</v>
-      </c>
-      <c r="G37" s="36">
-        <v>0</v>
-      </c>
-      <c r="H37" s="37">
+      <c r="D37" s="34">
+        <v>0</v>
+      </c>
+      <c r="E37" s="35">
+        <v>0</v>
+      </c>
+      <c r="F37" s="35">
+        <v>0</v>
+      </c>
+      <c r="G37" s="35">
+        <v>0</v>
+      </c>
+      <c r="H37" s="36">
         <v>500</v>
       </c>
       <c r="J37" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="K37" s="49">
-        <v>0</v>
-      </c>
-      <c r="L37" s="50">
+      <c r="K37" s="48">
+        <v>0</v>
+      </c>
+      <c r="L37" s="49">
         <v>500</v>
       </c>
-      <c r="M37" s="51">
+      <c r="M37" s="50">
         <f>50%*500</f>
         <v>250</v>
       </c>
-      <c r="N37" s="25"/>
+      <c r="N37" s="24"/>
       <c r="O37" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="P37" s="51">
+      <c r="P37" s="50">
         <f t="shared" si="3"/>
         <v>750</v>
       </c>
       <c r="R37" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="S37" s="54">
+      <c r="S37" s="51">
         <f>-P37/$H$41</f>
         <v>-1.5000000000000004</v>
       </c>
-      <c r="T37" s="66"/>
+      <c r="T37" s="63"/>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B38" s="65"/>
-      <c r="N38" s="25"/>
-      <c r="T38" s="66"/>
+      <c r="B38" s="62"/>
+      <c r="N38" s="24"/>
+      <c r="T38" s="63"/>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B39" s="65"/>
+      <c r="B39" s="62"/>
       <c r="D39" s="1" t="s">
         <v>16</v>
       </c>
@@ -2801,27 +2792,27 @@
         <v>16</v>
       </c>
       <c r="L39" s="1"/>
-      <c r="N39" s="25"/>
-      <c r="T39" s="66"/>
+      <c r="N39" s="24"/>
+      <c r="T39" s="63"/>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B40" s="65"/>
-      <c r="D40" s="26" t="s">
+      <c r="B40" s="62"/>
+      <c r="D40" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E40" s="27" t="s">
+      <c r="E40" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="F40" s="27" t="s">
+      <c r="F40" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="G40" s="27" t="s">
+      <c r="G40" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="H40" s="28" t="s">
+      <c r="H40" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="K40" s="26" t="s">
+      <c r="K40" s="25" t="s">
         <v>11</v>
       </c>
       <c r="L40" s="11" t="s">
@@ -2830,78 +2821,78 @@
       <c r="M40" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="N40" s="25"/>
-      <c r="O40" s="25"/>
-      <c r="P40" s="61" t="s">
+      <c r="N40" s="24"/>
+      <c r="O40" s="24"/>
+      <c r="P40" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="T40" s="66"/>
+      <c r="T40" s="63"/>
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B41" s="65"/>
-      <c r="D41" s="35">
+      <c r="B41" s="62"/>
+      <c r="D41" s="34">
         <f t="shared" ref="D41:H41" si="4">SUM(D28:D37)</f>
         <v>100</v>
       </c>
-      <c r="E41" s="36">
+      <c r="E41" s="35">
         <f t="shared" si="4"/>
         <v>200</v>
       </c>
-      <c r="F41" s="36">
+      <c r="F41" s="35">
         <f t="shared" si="4"/>
         <v>299.99999999999983</v>
       </c>
-      <c r="G41" s="36">
+      <c r="G41" s="35">
         <f t="shared" si="4"/>
         <v>399.99999999999989</v>
       </c>
-      <c r="H41" s="37">
+      <c r="H41" s="36">
         <f t="shared" si="4"/>
         <v>499.99999999999989</v>
       </c>
-      <c r="K41" s="55">
+      <c r="K41" s="52">
         <f t="shared" ref="K41" si="5">SUM(K28:K37)</f>
         <v>100</v>
       </c>
-      <c r="L41" s="55">
+      <c r="L41" s="52">
         <f>SUM(L28:L37)</f>
         <v>100</v>
       </c>
-      <c r="M41" s="56">
+      <c r="M41" s="53">
         <f>SUM(M28:M37)</f>
         <v>449.99999999999989</v>
       </c>
-      <c r="N41" s="25"/>
-      <c r="P41" s="56">
+      <c r="N41" s="24"/>
+      <c r="P41" s="53">
         <f>SUM(P28:P37)</f>
         <v>649.99999999999989</v>
       </c>
-      <c r="T41" s="66"/>
+      <c r="T41" s="63"/>
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B42" s="65"/>
-      <c r="T42" s="66"/>
+      <c r="B42" s="62"/>
+      <c r="T42" s="63"/>
     </row>
     <row r="43" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B43" s="67"/>
-      <c r="C43" s="68"/>
-      <c r="D43" s="68"/>
-      <c r="E43" s="68"/>
-      <c r="F43" s="68"/>
-      <c r="G43" s="68"/>
-      <c r="H43" s="68"/>
-      <c r="I43" s="68"/>
-      <c r="J43" s="68"/>
-      <c r="K43" s="68"/>
-      <c r="L43" s="68"/>
-      <c r="M43" s="68"/>
-      <c r="N43" s="68"/>
-      <c r="O43" s="68"/>
-      <c r="P43" s="68"/>
-      <c r="Q43" s="68"/>
-      <c r="R43" s="68"/>
-      <c r="S43" s="68"/>
-      <c r="T43" s="70"/>
+      <c r="B43" s="64"/>
+      <c r="C43" s="65"/>
+      <c r="D43" s="65"/>
+      <c r="E43" s="65"/>
+      <c r="F43" s="65"/>
+      <c r="G43" s="65"/>
+      <c r="H43" s="65"/>
+      <c r="I43" s="65"/>
+      <c r="J43" s="65"/>
+      <c r="K43" s="65"/>
+      <c r="L43" s="65"/>
+      <c r="M43" s="65"/>
+      <c r="N43" s="65"/>
+      <c r="O43" s="65"/>
+      <c r="P43" s="65"/>
+      <c r="Q43" s="65"/>
+      <c r="R43" s="65"/>
+      <c r="S43" s="65"/>
+      <c r="T43" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Updating Fast Risk / Trader Rules of Thumb
</commit_message>
<xml_diff>
--- a/11 Trader Rules of Thumb/TraderTricks.xlsx
+++ b/11 Trader Rules of Thumb/TraderTricks.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\BOOK\.SWAPS_BOOK\11 Trader Rules of Thumb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251E5BB2-798E-4B79-BF74-361F85DE153B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26711D65-AFA0-46FC-B655-9D434C689DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{2C45AD73-A93A-4DE3-9C06-A85BD7C29742}"/>
+    <workbookView xWindow="18765" yWindow="2685" windowWidth="22620" windowHeight="15345" xr2:uid="{2C45AD73-A93A-4DE3-9C06-A85BD7C29742}"/>
   </bookViews>
   <sheets>
     <sheet name="Trick 1 - Quick Risk" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029" calcCompleted="0" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -651,7 +651,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -834,6 +834,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="7" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1285,7 +1291,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1943,8 +1949,8 @@
       <c r="R15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="S15" s="17">
-        <f>-P15/$G$20</f>
+      <c r="S15" s="72">
+        <f ca="1">-P15/$G$20</f>
         <v>0.50000000000000011</v>
       </c>
       <c r="T15" s="63"/>
@@ -2722,7 +2728,7 @@
       <c r="R36" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="S36" s="47">
+      <c r="S36" s="73">
         <f>-P36/$G$41</f>
         <v>0.50000000000000011</v>
       </c>

</xml_diff>